<commit_message>
Pruebas sin nodos auxiliares
</commit_message>
<xml_diff>
--- a/files/prediction_output_analisis.xlsx
+++ b/files/prediction_output_analisis.xlsx
@@ -3351,11 +3351,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -3371,6 +3372,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3415,12 +3421,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3535,6 +3549,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -4143,6 +4158,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -4748,6 +4764,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -5335,17 +5352,17 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="40763301"/>
-        <c:axId val="5088763"/>
+        <c:axId val="92568505"/>
+        <c:axId val="84927840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40763301"/>
+        <c:axId val="92568505"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5367,7 +5384,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5088763"/>
+        <c:crossAx val="84927840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5375,7 +5392,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="5088763"/>
+        <c:axId val="84927840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5390,7 +5407,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5412,7 +5429,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40763301"/>
+        <c:crossAx val="92568505"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5447,7 +5464,7 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -5465,15 +5482,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>875160</xdr:colOff>
+      <xdr:colOff>865440</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>57600</xdr:rowOff>
+      <xdr:rowOff>47880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>710640</xdr:colOff>
+      <xdr:colOff>700560</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>48240</xdr:rowOff>
+      <xdr:rowOff>38160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5481,8 +5498,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8488080" y="219960"/>
-        <a:ext cx="5760720" cy="3241800"/>
+        <a:off x="8476920" y="210240"/>
+        <a:ext cx="5767920" cy="3241440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5503,16 +5520,16 @@
   <dimension ref="A1:N186"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N30" activeCellId="0" sqref="N30"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="10.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="1" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.86"/>
   </cols>
   <sheetData>
@@ -5535,13 +5552,13 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5555,22 +5572,22 @@
       <c r="C2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>1.1166277</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="1" t="n">
         <v>3.4590275</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="1" t="n">
         <v>0.103538275</v>
       </c>
     </row>
@@ -5593,13 +5610,13 @@
       <c r="F3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>0.7624264</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="1" t="n">
         <v>3.9202573</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="1" t="n">
         <v>0.07723224</v>
       </c>
     </row>
@@ -5622,13 +5639,13 @@
       <c r="F4" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>0.14616203</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="1" t="n">
         <v>0.16954851</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="1" t="n">
         <v>0.066747904</v>
       </c>
     </row>
@@ -5651,13 +5668,13 @@
       <c r="F5" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <v>0.858902</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="1" t="n">
         <v>0.9281802</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="I5" s="1" t="n">
         <v>0.104693174</v>
       </c>
     </row>
@@ -5680,13 +5697,13 @@
       <c r="F6" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <v>2.4001198</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="1" t="n">
         <v>2.0243325</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="I6" s="1" t="n">
         <v>0.10340679</v>
       </c>
     </row>
@@ -5709,13 +5726,13 @@
       <c r="F7" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>1.1493912</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7" s="1" t="n">
         <v>3.079526</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="I7" s="1" t="n">
         <v>0.10453534</v>
       </c>
     </row>
@@ -5732,19 +5749,19 @@
       <c r="D8" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <v>3.232664</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="I8" s="1" t="n">
         <v>0.09255159</v>
       </c>
     </row>
@@ -5767,13 +5784,13 @@
       <c r="F9" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>0.9183855</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="1" t="n">
         <v>1.8175483</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="I9" s="1" t="n">
         <v>0.14555395</v>
       </c>
     </row>
@@ -5796,13 +5813,13 @@
       <c r="F10" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>0.96157265</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="1" t="n">
         <v>0.5513511</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="I10" s="1" t="n">
         <v>0.12113297</v>
       </c>
     </row>
@@ -5825,13 +5842,13 @@
       <c r="F11" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="1" t="n">
         <v>4.3482056</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11" s="1" t="n">
         <v>4.0491047</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="I11" s="1" t="n">
         <v>0.09493375</v>
       </c>
     </row>
@@ -5854,13 +5871,13 @@
       <c r="F12" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="1" t="n">
         <v>1.300642</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12" s="1" t="n">
         <v>4.063759</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="I12" s="1" t="n">
         <v>0.09445238</v>
       </c>
     </row>
@@ -5883,13 +5900,13 @@
       <c r="F13" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="1" t="n">
         <v>1.437253</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="H13" s="1" t="n">
         <v>4.070363</v>
       </c>
-      <c r="I13" s="0" t="n">
+      <c r="I13" s="1" t="n">
         <v>0.12497103</v>
       </c>
     </row>
@@ -5909,16 +5926,16 @@
       <c r="E14" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="1" t="n">
         <v>0.87789345</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="H14" s="1" t="n">
         <v>1.8716455</v>
       </c>
-      <c r="I14" s="0" t="n">
+      <c r="I14" s="1" t="n">
         <v>0.1421647</v>
       </c>
     </row>
@@ -5938,16 +5955,16 @@
       <c r="E15" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="1" t="n">
         <v>1.8771944</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15" s="1" t="n">
         <v>2.859036</v>
       </c>
-      <c r="I15" s="0" t="n">
+      <c r="I15" s="1" t="n">
         <v>0.15359807</v>
       </c>
     </row>
@@ -5970,13 +5987,13 @@
       <c r="F16" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="1" t="n">
         <v>2.08325</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="H16" s="1" t="n">
         <v>2.4070563</v>
       </c>
-      <c r="I16" s="0" t="n">
+      <c r="I16" s="1" t="n">
         <v>0.12170863</v>
       </c>
     </row>
@@ -5999,13 +6016,13 @@
       <c r="F17" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="1" t="n">
         <v>0.26446724</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="H17" s="1" t="n">
         <v>0.027185917</v>
       </c>
-      <c r="I17" s="0" t="n">
+      <c r="I17" s="1" t="n">
         <v>0.08715224</v>
       </c>
     </row>
@@ -6028,13 +6045,13 @@
       <c r="F18" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="G18" s="1" t="n">
         <v>1.1734657</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="H18" s="1" t="n">
         <v>0.19540763</v>
       </c>
-      <c r="I18" s="0" t="n">
+      <c r="I18" s="1" t="n">
         <v>0.09817088</v>
       </c>
     </row>
@@ -6051,19 +6068,19 @@
       <c r="D19" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="G19" s="0" t="n">
+      <c r="G19" s="1" t="n">
         <v>0.2719078</v>
       </c>
-      <c r="H19" s="0" t="n">
+      <c r="H19" s="1" t="n">
         <v>0.037967205</v>
       </c>
-      <c r="I19" s="0" t="n">
+      <c r="I19" s="1" t="n">
         <v>0.0962311</v>
       </c>
     </row>
@@ -6083,16 +6100,16 @@
       <c r="E20" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="G20" s="1" t="n">
         <v>6.480136</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="H20" s="1" t="n">
         <v>5.8074007</v>
       </c>
-      <c r="I20" s="0" t="n">
+      <c r="I20" s="1" t="n">
         <v>0.052058697</v>
       </c>
     </row>
@@ -6109,19 +6126,19 @@
       <c r="D21" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="2" t="s">
         <v>125</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="G21" s="0" t="n">
+      <c r="G21" s="1" t="n">
         <v>0.11092663</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="H21" s="1" t="n">
         <v>0.36289978</v>
       </c>
-      <c r="I21" s="0" t="n">
+      <c r="I21" s="1" t="n">
         <v>0.043380618</v>
       </c>
     </row>
@@ -6144,13 +6161,13 @@
       <c r="F22" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="G22" s="0" t="n">
+      <c r="G22" s="1" t="n">
         <v>3.0073252</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="H22" s="1" t="n">
         <v>1.2564778</v>
       </c>
-      <c r="I22" s="0" t="n">
+      <c r="I22" s="1" t="n">
         <v>0.06943631</v>
       </c>
     </row>
@@ -6173,13 +6190,13 @@
       <c r="F23" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="G23" s="0" t="n">
+      <c r="G23" s="1" t="n">
         <v>1.0572662</v>
       </c>
-      <c r="H23" s="0" t="n">
+      <c r="H23" s="1" t="n">
         <v>1.0077367</v>
       </c>
-      <c r="I23" s="0" t="n">
+      <c r="I23" s="1" t="n">
         <v>0.13447559</v>
       </c>
     </row>
@@ -6202,13 +6219,13 @@
       <c r="F24" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="G24" s="0" t="n">
+      <c r="G24" s="1" t="n">
         <v>2.2892199</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="H24" s="1" t="n">
         <v>2.769444</v>
       </c>
-      <c r="I24" s="0" t="n">
+      <c r="I24" s="1" t="n">
         <v>0.09252584</v>
       </c>
       <c r="L24" s="0" t="s">
@@ -6240,13 +6257,13 @@
       <c r="F25" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="G25" s="1" t="n">
         <v>0.65323925</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="H25" s="1" t="n">
         <v>2.9666262</v>
       </c>
-      <c r="I25" s="0" t="n">
+      <c r="I25" s="1" t="n">
         <v>0.07375026</v>
       </c>
       <c r="K25" s="0" t="s">
@@ -6284,13 +6301,13 @@
       <c r="F26" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="G26" s="0" t="n">
+      <c r="G26" s="1" t="n">
         <v>0.23291016</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="H26" s="1" t="n">
         <v>1.3828404</v>
       </c>
-      <c r="I26" s="0" t="n">
+      <c r="I26" s="1" t="n">
         <v>0.108113885</v>
       </c>
       <c r="K26" s="0" t="s">
@@ -6328,13 +6345,13 @@
       <c r="F27" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="G27" s="0" t="n">
+      <c r="G27" s="1" t="n">
         <v>1.5318623</v>
       </c>
-      <c r="H27" s="0" t="n">
+      <c r="H27" s="1" t="n">
         <v>0.62613773</v>
       </c>
-      <c r="I27" s="0" t="n">
+      <c r="I27" s="1" t="n">
         <v>0.13936162</v>
       </c>
       <c r="K27" s="0" t="s">
@@ -6372,13 +6389,13 @@
       <c r="F28" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="G28" s="0" t="n">
+      <c r="G28" s="1" t="n">
         <v>4.763484</v>
       </c>
-      <c r="H28" s="0" t="n">
+      <c r="H28" s="1" t="n">
         <v>0.7322302</v>
       </c>
-      <c r="I28" s="0" t="n">
+      <c r="I28" s="1" t="n">
         <v>0.09862268</v>
       </c>
     </row>
@@ -6401,13 +6418,13 @@
       <c r="F29" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="G29" s="0" t="n">
+      <c r="G29" s="1" t="n">
         <v>5.406843</v>
       </c>
-      <c r="H29" s="0" t="n">
+      <c r="H29" s="1" t="n">
         <v>1.208642</v>
       </c>
-      <c r="I29" s="0" t="n">
+      <c r="I29" s="1" t="n">
         <v>0.08948326</v>
       </c>
     </row>
@@ -6430,13 +6447,13 @@
       <c r="F30" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="G30" s="0" t="n">
+      <c r="G30" s="1" t="n">
         <v>2.9322786</v>
       </c>
-      <c r="H30" s="0" t="n">
+      <c r="H30" s="1" t="n">
         <v>1.9464812</v>
       </c>
-      <c r="I30" s="0" t="n">
+      <c r="I30" s="1" t="n">
         <v>0.11972463</v>
       </c>
     </row>
@@ -6459,13 +6476,13 @@
       <c r="F31" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="G31" s="0" t="n">
+      <c r="G31" s="1" t="n">
         <v>0.48657322</v>
       </c>
-      <c r="H31" s="0" t="n">
+      <c r="H31" s="1" t="n">
         <v>2.8339992</v>
       </c>
-      <c r="I31" s="0" t="n">
+      <c r="I31" s="1" t="n">
         <v>0.145895</v>
       </c>
     </row>
@@ -6488,13 +6505,13 @@
       <c r="F32" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="G32" s="0" t="n">
+      <c r="G32" s="1" t="n">
         <v>0.15931511</v>
       </c>
-      <c r="H32" s="0" t="n">
+      <c r="H32" s="1" t="n">
         <v>0.5779474</v>
       </c>
-      <c r="I32" s="0" t="n">
+      <c r="I32" s="1" t="n">
         <v>0.16301453</v>
       </c>
     </row>
@@ -6514,16 +6531,16 @@
       <c r="E33" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F33" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="G33" s="0" t="n">
+      <c r="G33" s="1" t="n">
         <v>5.075842</v>
       </c>
-      <c r="H33" s="0" t="n">
+      <c r="H33" s="1" t="n">
         <v>4.210153</v>
       </c>
-      <c r="I33" s="0" t="n">
+      <c r="I33" s="1" t="n">
         <v>0.06763852</v>
       </c>
     </row>
@@ -6546,13 +6563,13 @@
       <c r="F34" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="G34" s="0" t="n">
+      <c r="G34" s="1" t="n">
         <v>4.682398</v>
       </c>
-      <c r="H34" s="0" t="n">
+      <c r="H34" s="1" t="n">
         <v>1.1110516</v>
       </c>
-      <c r="I34" s="0" t="n">
+      <c r="I34" s="1" t="n">
         <v>0.106456995</v>
       </c>
     </row>
@@ -6575,13 +6592,13 @@
       <c r="F35" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="G35" s="0" t="n">
+      <c r="G35" s="1" t="n">
         <v>2.1556816</v>
       </c>
-      <c r="H35" s="0" t="n">
+      <c r="H35" s="1" t="n">
         <v>1.0448594</v>
       </c>
-      <c r="I35" s="0" t="n">
+      <c r="I35" s="1" t="n">
         <v>0.14072967</v>
       </c>
     </row>
@@ -6604,13 +6621,13 @@
       <c r="F36" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="G36" s="0" t="n">
+      <c r="G36" s="1" t="n">
         <v>3.2483706</v>
       </c>
-      <c r="H36" s="0" t="n">
+      <c r="H36" s="1" t="n">
         <v>1.4580886</v>
       </c>
-      <c r="I36" s="0" t="n">
+      <c r="I36" s="1" t="n">
         <v>0.17357314</v>
       </c>
     </row>
@@ -6627,19 +6644,19 @@
       <c r="D37" s="0" t="s">
         <v>225</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="2" t="s">
         <v>226</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="G37" s="0" t="n">
+      <c r="G37" s="1" t="n">
         <v>6.096961</v>
       </c>
-      <c r="H37" s="0" t="n">
+      <c r="H37" s="1" t="n">
         <v>3.759016</v>
       </c>
-      <c r="I37" s="0" t="n">
+      <c r="I37" s="1" t="n">
         <v>0.09901309</v>
       </c>
     </row>
@@ -6662,13 +6679,13 @@
       <c r="F38" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="G38" s="0" t="n">
+      <c r="G38" s="1" t="n">
         <v>3.187821</v>
       </c>
-      <c r="H38" s="0" t="n">
+      <c r="H38" s="1" t="n">
         <v>1.0615506</v>
       </c>
-      <c r="I38" s="0" t="n">
+      <c r="I38" s="1" t="n">
         <v>0.124318</v>
       </c>
     </row>
@@ -6691,13 +6708,13 @@
       <c r="F39" s="0" t="s">
         <v>239</v>
       </c>
-      <c r="G39" s="0" t="n">
+      <c r="G39" s="1" t="n">
         <v>7.989081</v>
       </c>
-      <c r="H39" s="0" t="n">
+      <c r="H39" s="1" t="n">
         <v>1.0315068</v>
       </c>
-      <c r="I39" s="0" t="n">
+      <c r="I39" s="1" t="n">
         <v>0.11803019</v>
       </c>
     </row>
@@ -6720,13 +6737,13 @@
       <c r="F40" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="G40" s="0" t="n">
+      <c r="G40" s="1" t="n">
         <v>3.8049998</v>
       </c>
-      <c r="H40" s="0" t="n">
+      <c r="H40" s="1" t="n">
         <v>0.254663</v>
       </c>
-      <c r="I40" s="0" t="n">
+      <c r="I40" s="1" t="n">
         <v>0.18657684</v>
       </c>
     </row>
@@ -6749,13 +6766,13 @@
       <c r="F41" s="0" t="s">
         <v>251</v>
       </c>
-      <c r="G41" s="0" t="n">
+      <c r="G41" s="1" t="n">
         <v>0.42490387</v>
       </c>
-      <c r="H41" s="0" t="n">
+      <c r="H41" s="1" t="n">
         <v>2.2289004</v>
       </c>
-      <c r="I41" s="0" t="n">
+      <c r="I41" s="1" t="n">
         <v>0.088217735</v>
       </c>
     </row>
@@ -6772,19 +6789,19 @@
       <c r="D42" s="0" t="s">
         <v>255</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" s="2" t="s">
         <v>256</v>
       </c>
       <c r="F42" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="G42" s="0" t="n">
+      <c r="G42" s="1" t="n">
         <v>5.274277</v>
       </c>
-      <c r="H42" s="0" t="n">
+      <c r="H42" s="1" t="n">
         <v>2.18844</v>
       </c>
-      <c r="I42" s="0" t="n">
+      <c r="I42" s="1" t="n">
         <v>0.14305401</v>
       </c>
     </row>
@@ -6807,13 +6824,13 @@
       <c r="F43" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="G43" s="0" t="n">
+      <c r="G43" s="1" t="n">
         <v>2.3391385</v>
       </c>
-      <c r="H43" s="0" t="n">
+      <c r="H43" s="1" t="n">
         <v>2.5422</v>
       </c>
-      <c r="I43" s="0" t="n">
+      <c r="I43" s="1" t="n">
         <v>0.21485913</v>
       </c>
     </row>
@@ -6836,13 +6853,13 @@
       <c r="F44" s="0" t="s">
         <v>269</v>
       </c>
-      <c r="G44" s="0" t="n">
+      <c r="G44" s="1" t="n">
         <v>8.271671</v>
       </c>
-      <c r="H44" s="0" t="n">
+      <c r="H44" s="1" t="n">
         <v>2.1373825</v>
       </c>
-      <c r="I44" s="0" t="n">
+      <c r="I44" s="1" t="n">
         <v>0.060421586</v>
       </c>
     </row>
@@ -6865,13 +6882,13 @@
       <c r="F45" s="0" t="s">
         <v>275</v>
       </c>
-      <c r="G45" s="0" t="n">
+      <c r="G45" s="1" t="n">
         <v>3.96281</v>
       </c>
-      <c r="H45" s="0" t="n">
+      <c r="H45" s="1" t="n">
         <v>0.0792613</v>
       </c>
-      <c r="I45" s="0" t="n">
+      <c r="I45" s="1" t="n">
         <v>0.17120469</v>
       </c>
     </row>
@@ -6894,13 +6911,13 @@
       <c r="F46" s="0" t="s">
         <v>281</v>
       </c>
-      <c r="G46" s="0" t="n">
+      <c r="G46" s="1" t="n">
         <v>4.866548</v>
       </c>
-      <c r="H46" s="0" t="n">
+      <c r="H46" s="1" t="n">
         <v>0.88978076</v>
       </c>
-      <c r="I46" s="0" t="n">
+      <c r="I46" s="1" t="n">
         <v>0.2597313</v>
       </c>
     </row>
@@ -6923,13 +6940,13 @@
       <c r="F47" s="0" t="s">
         <v>287</v>
       </c>
-      <c r="G47" s="0" t="n">
+      <c r="G47" s="1" t="n">
         <v>5.892816</v>
       </c>
-      <c r="H47" s="0" t="n">
+      <c r="H47" s="1" t="n">
         <v>1.3621614</v>
       </c>
-      <c r="I47" s="0" t="n">
+      <c r="I47" s="1" t="n">
         <v>0.26754224</v>
       </c>
     </row>
@@ -6952,13 +6969,13 @@
       <c r="F48" s="0" t="s">
         <v>293</v>
       </c>
-      <c r="G48" s="0" t="n">
+      <c r="G48" s="1" t="n">
         <v>6.03959</v>
       </c>
-      <c r="H48" s="0" t="n">
+      <c r="H48" s="1" t="n">
         <v>3.2935872</v>
       </c>
-      <c r="I48" s="0" t="n">
+      <c r="I48" s="1" t="n">
         <v>0.22724414</v>
       </c>
     </row>
@@ -6981,13 +6998,13 @@
       <c r="F49" s="0" t="s">
         <v>299</v>
       </c>
-      <c r="G49" s="0" t="n">
+      <c r="G49" s="1" t="n">
         <v>0.24115133</v>
       </c>
-      <c r="H49" s="0" t="n">
+      <c r="H49" s="1" t="n">
         <v>0.8751192</v>
       </c>
-      <c r="I49" s="0" t="n">
+      <c r="I49" s="1" t="n">
         <v>0.15704548</v>
       </c>
     </row>
@@ -7010,13 +7027,13 @@
       <c r="F50" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="G50" s="0" t="n">
+      <c r="G50" s="1" t="n">
         <v>2.5040178</v>
       </c>
-      <c r="H50" s="0" t="n">
+      <c r="H50" s="1" t="n">
         <v>1.8135469</v>
       </c>
-      <c r="I50" s="0" t="n">
+      <c r="I50" s="1" t="n">
         <v>0.11378145</v>
       </c>
     </row>
@@ -7039,13 +7056,13 @@
       <c r="F51" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="G51" s="0" t="n">
+      <c r="G51" s="1" t="n">
         <v>4.733361</v>
       </c>
-      <c r="H51" s="0" t="n">
+      <c r="H51" s="1" t="n">
         <v>4.4044437</v>
       </c>
-      <c r="I51" s="0" t="n">
+      <c r="I51" s="1" t="n">
         <v>0.09424281</v>
       </c>
     </row>
@@ -7062,19 +7079,19 @@
       <c r="D52" s="0" t="s">
         <v>314</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E52" s="2" t="s">
         <v>315</v>
       </c>
       <c r="F52" s="0" t="s">
         <v>316</v>
       </c>
-      <c r="G52" s="0" t="n">
+      <c r="G52" s="1" t="n">
         <v>3.9985785</v>
       </c>
-      <c r="H52" s="0" t="n">
+      <c r="H52" s="1" t="n">
         <v>1.6569536</v>
       </c>
-      <c r="I52" s="0" t="n">
+      <c r="I52" s="1" t="n">
         <v>0.06881869</v>
       </c>
     </row>
@@ -7097,13 +7114,13 @@
       <c r="F53" s="0" t="s">
         <v>322</v>
       </c>
-      <c r="G53" s="0" t="n">
+      <c r="G53" s="1" t="n">
         <v>3.1197252</v>
       </c>
-      <c r="H53" s="0" t="n">
+      <c r="H53" s="1" t="n">
         <v>0.34606075</v>
       </c>
-      <c r="I53" s="0" t="n">
+      <c r="I53" s="1" t="n">
         <v>0.14906359</v>
       </c>
     </row>
@@ -7126,13 +7143,13 @@
       <c r="F54" s="0" t="s">
         <v>328</v>
       </c>
-      <c r="G54" s="0" t="n">
+      <c r="G54" s="1" t="n">
         <v>8.933924</v>
       </c>
-      <c r="H54" s="0" t="n">
+      <c r="H54" s="1" t="n">
         <v>0.49946117</v>
       </c>
-      <c r="I54" s="0" t="n">
+      <c r="I54" s="1" t="n">
         <v>0.11974287</v>
       </c>
     </row>
@@ -7155,13 +7172,13 @@
       <c r="F55" s="0" t="s">
         <v>334</v>
       </c>
-      <c r="G55" s="0" t="n">
+      <c r="G55" s="1" t="n">
         <v>1.1129847</v>
       </c>
-      <c r="H55" s="0" t="n">
+      <c r="H55" s="1" t="n">
         <v>0.012226582</v>
       </c>
-      <c r="I55" s="0" t="n">
+      <c r="I55" s="1" t="n">
         <v>0.16135573</v>
       </c>
     </row>
@@ -7184,13 +7201,13 @@
       <c r="F56" s="0" t="s">
         <v>340</v>
       </c>
-      <c r="G56" s="0" t="n">
+      <c r="G56" s="1" t="n">
         <v>11.139456</v>
       </c>
-      <c r="H56" s="0" t="n">
+      <c r="H56" s="1" t="n">
         <v>1.3277717</v>
       </c>
-      <c r="I56" s="0" t="n">
+      <c r="I56" s="1" t="n">
         <v>0.14669931</v>
       </c>
     </row>
@@ -7213,13 +7230,13 @@
       <c r="F57" s="0" t="s">
         <v>345</v>
       </c>
-      <c r="G57" s="0" t="n">
+      <c r="G57" s="1" t="n">
         <v>5.7881007</v>
       </c>
-      <c r="H57" s="0" t="n">
+      <c r="H57" s="1" t="n">
         <v>3.6673498</v>
       </c>
-      <c r="I57" s="0" t="n">
+      <c r="I57" s="1" t="n">
         <v>0.20578778</v>
       </c>
     </row>
@@ -7242,13 +7259,13 @@
       <c r="F58" s="0" t="s">
         <v>351</v>
       </c>
-      <c r="G58" s="0" t="n">
+      <c r="G58" s="1" t="n">
         <v>1.7432864</v>
       </c>
-      <c r="H58" s="0" t="n">
+      <c r="H58" s="1" t="n">
         <v>1.1596789</v>
       </c>
-      <c r="I58" s="0" t="n">
+      <c r="I58" s="1" t="n">
         <v>0.2293812</v>
       </c>
     </row>
@@ -7271,13 +7288,13 @@
       <c r="F59" s="0" t="s">
         <v>357</v>
       </c>
-      <c r="G59" s="0" t="n">
+      <c r="G59" s="1" t="n">
         <v>2.4753299</v>
       </c>
-      <c r="H59" s="0" t="n">
+      <c r="H59" s="1" t="n">
         <v>1.8443289</v>
       </c>
-      <c r="I59" s="0" t="n">
+      <c r="I59" s="1" t="n">
         <v>0.24260819</v>
       </c>
     </row>
@@ -7300,13 +7317,13 @@
       <c r="F60" s="0" t="s">
         <v>363</v>
       </c>
-      <c r="G60" s="0" t="n">
+      <c r="G60" s="1" t="n">
         <v>0.09563637</v>
       </c>
-      <c r="H60" s="0" t="n">
+      <c r="H60" s="1" t="n">
         <v>2.2322564</v>
       </c>
-      <c r="I60" s="0" t="n">
+      <c r="I60" s="1" t="n">
         <v>0.24474835</v>
       </c>
     </row>
@@ -7329,13 +7346,13 @@
       <c r="F61" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="G61" s="0" t="n">
+      <c r="G61" s="1" t="n">
         <v>2.9021807</v>
       </c>
-      <c r="H61" s="0" t="n">
+      <c r="H61" s="1" t="n">
         <v>0.674273</v>
       </c>
-      <c r="I61" s="0" t="n">
+      <c r="I61" s="1" t="n">
         <v>0.22462296</v>
       </c>
     </row>
@@ -7358,13 +7375,13 @@
       <c r="F62" s="0" t="s">
         <v>375</v>
       </c>
-      <c r="G62" s="0" t="n">
+      <c r="G62" s="1" t="n">
         <v>2.1446936</v>
       </c>
-      <c r="H62" s="0" t="n">
+      <c r="H62" s="1" t="n">
         <v>1.4223671</v>
       </c>
-      <c r="I62" s="0" t="n">
+      <c r="I62" s="1" t="n">
         <v>0.123278975</v>
       </c>
     </row>
@@ -7387,13 +7404,13 @@
       <c r="F63" s="0" t="s">
         <v>380</v>
       </c>
-      <c r="G63" s="0" t="n">
+      <c r="G63" s="1" t="n">
         <v>5.5674157</v>
       </c>
-      <c r="H63" s="0" t="n">
+      <c r="H63" s="1" t="n">
         <v>1.1179361</v>
       </c>
-      <c r="I63" s="0" t="n">
+      <c r="I63" s="1" t="n">
         <v>0.1142472</v>
       </c>
     </row>
@@ -7416,13 +7433,13 @@
       <c r="F64" s="0" t="s">
         <v>386</v>
       </c>
-      <c r="G64" s="0" t="n">
+      <c r="G64" s="1" t="n">
         <v>4.6121817</v>
       </c>
-      <c r="H64" s="0" t="n">
+      <c r="H64" s="1" t="n">
         <v>0.90145254</v>
       </c>
-      <c r="I64" s="0" t="n">
+      <c r="I64" s="1" t="n">
         <v>0.2048788</v>
       </c>
     </row>
@@ -7445,13 +7462,13 @@
       <c r="F65" s="0" t="s">
         <v>392</v>
       </c>
-      <c r="G65" s="0" t="n">
+      <c r="G65" s="1" t="n">
         <v>5.3782105</v>
       </c>
-      <c r="H65" s="0" t="n">
+      <c r="H65" s="1" t="n">
         <v>0.6017337</v>
       </c>
-      <c r="I65" s="0" t="n">
+      <c r="I65" s="1" t="n">
         <v>0.11341488</v>
       </c>
     </row>
@@ -7474,13 +7491,13 @@
       <c r="F66" s="0" t="s">
         <v>398</v>
       </c>
-      <c r="G66" s="0" t="n">
+      <c r="G66" s="1" t="n">
         <v>0.9656215</v>
       </c>
-      <c r="H66" s="0" t="n">
+      <c r="H66" s="1" t="n">
         <v>0.99591446</v>
       </c>
-      <c r="I66" s="0" t="n">
+      <c r="I66" s="1" t="n">
         <v>0.14180744</v>
       </c>
     </row>
@@ -7503,13 +7520,13 @@
       <c r="F67" s="0" t="s">
         <v>403</v>
       </c>
-      <c r="G67" s="0" t="n">
+      <c r="G67" s="1" t="n">
         <v>5.681526</v>
       </c>
-      <c r="H67" s="0" t="n">
+      <c r="H67" s="1" t="n">
         <v>1.4113164</v>
       </c>
-      <c r="I67" s="0" t="n">
+      <c r="I67" s="1" t="n">
         <v>0.14233458</v>
       </c>
     </row>
@@ -7532,13 +7549,13 @@
       <c r="F68" s="0" t="s">
         <v>409</v>
       </c>
-      <c r="G68" s="0" t="n">
+      <c r="G68" s="1" t="n">
         <v>1.4166574</v>
       </c>
-      <c r="H68" s="0" t="n">
+      <c r="H68" s="1" t="n">
         <v>2.3668685</v>
       </c>
-      <c r="I68" s="0" t="n">
+      <c r="I68" s="1" t="n">
         <v>0.14305949</v>
       </c>
     </row>
@@ -7561,13 +7578,13 @@
       <c r="F69" s="0" t="s">
         <v>414</v>
       </c>
-      <c r="G69" s="0" t="n">
+      <c r="G69" s="1" t="n">
         <v>5.700862</v>
       </c>
-      <c r="H69" s="0" t="n">
+      <c r="H69" s="1" t="n">
         <v>3.0675092</v>
       </c>
-      <c r="I69" s="0" t="n">
+      <c r="I69" s="1" t="n">
         <v>0.14703977</v>
       </c>
     </row>
@@ -7590,13 +7607,13 @@
       <c r="F70" s="0" t="s">
         <v>420</v>
       </c>
-      <c r="G70" s="0" t="n">
+      <c r="G70" s="1" t="n">
         <v>1.3996286</v>
       </c>
-      <c r="H70" s="0" t="n">
+      <c r="H70" s="1" t="n">
         <v>3.4396467</v>
       </c>
-      <c r="I70" s="0" t="n">
+      <c r="I70" s="1" t="n">
         <v>0.12514794</v>
       </c>
     </row>
@@ -7616,16 +7633,16 @@
       <c r="E71" s="0" t="s">
         <v>425</v>
       </c>
-      <c r="F71" s="1" t="s">
+      <c r="F71" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="G71" s="0" t="n">
+      <c r="G71" s="1" t="n">
         <v>0.35037947</v>
       </c>
-      <c r="H71" s="0" t="n">
+      <c r="H71" s="1" t="n">
         <v>0.5837989</v>
       </c>
-      <c r="I71" s="0" t="n">
+      <c r="I71" s="1" t="n">
         <v>0.10663462</v>
       </c>
     </row>
@@ -7639,22 +7656,22 @@
       <c r="C72" s="0" t="s">
         <v>429</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D72" s="2" t="s">
         <v>430</v>
       </c>
       <c r="E72" s="0" t="s">
         <v>431</v>
       </c>
-      <c r="F72" s="1" t="s">
+      <c r="F72" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="G72" s="0" t="n">
+      <c r="G72" s="1" t="n">
         <v>3.9752648</v>
       </c>
-      <c r="H72" s="0" t="n">
+      <c r="H72" s="1" t="n">
         <v>0.58502483</v>
       </c>
-      <c r="I72" s="0" t="n">
+      <c r="I72" s="1" t="n">
         <v>0.115603805</v>
       </c>
     </row>
@@ -7677,13 +7694,13 @@
       <c r="F73" s="0" t="s">
         <v>438</v>
       </c>
-      <c r="G73" s="0" t="n">
+      <c r="G73" s="1" t="n">
         <v>5.4385448</v>
       </c>
-      <c r="H73" s="0" t="n">
+      <c r="H73" s="1" t="n">
         <v>0.29489326</v>
       </c>
-      <c r="I73" s="0" t="n">
+      <c r="I73" s="1" t="n">
         <v>0.14420974</v>
       </c>
     </row>
@@ -7706,13 +7723,13 @@
       <c r="F74" s="0" t="s">
         <v>444</v>
       </c>
-      <c r="G74" s="0" t="n">
+      <c r="G74" s="1" t="n">
         <v>3.6137638</v>
       </c>
-      <c r="H74" s="0" t="n">
+      <c r="H74" s="1" t="n">
         <v>1.3532043</v>
       </c>
-      <c r="I74" s="0" t="n">
+      <c r="I74" s="1" t="n">
         <v>0.12204301</v>
       </c>
     </row>
@@ -7726,7 +7743,7 @@
       <c r="C75" s="0" t="s">
         <v>447</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D75" s="2" t="s">
         <v>448</v>
       </c>
       <c r="E75" s="0" t="s">
@@ -7735,13 +7752,13 @@
       <c r="F75" s="0" t="s">
         <v>450</v>
       </c>
-      <c r="G75" s="0" t="n">
+      <c r="G75" s="1" t="n">
         <v>0.17500877</v>
       </c>
-      <c r="H75" s="0" t="n">
+      <c r="H75" s="1" t="n">
         <v>1.1402898</v>
       </c>
-      <c r="I75" s="0" t="n">
+      <c r="I75" s="1" t="n">
         <v>0.08752704</v>
       </c>
     </row>
@@ -7764,13 +7781,13 @@
       <c r="F76" s="0" t="s">
         <v>456</v>
       </c>
-      <c r="G76" s="0" t="n">
+      <c r="G76" s="1" t="n">
         <v>0.2107482</v>
       </c>
-      <c r="H76" s="0" t="n">
+      <c r="H76" s="1" t="n">
         <v>1.6700654</v>
       </c>
-      <c r="I76" s="0" t="n">
+      <c r="I76" s="1" t="n">
         <v>0.11303067</v>
       </c>
     </row>
@@ -7793,13 +7810,13 @@
       <c r="F77" s="0" t="s">
         <v>462</v>
       </c>
-      <c r="G77" s="0" t="n">
+      <c r="G77" s="1" t="n">
         <v>3.0728235</v>
       </c>
-      <c r="H77" s="0" t="n">
+      <c r="H77" s="1" t="n">
         <v>2.1931534</v>
       </c>
-      <c r="I77" s="0" t="n">
+      <c r="I77" s="1" t="n">
         <v>0.10880613</v>
       </c>
     </row>
@@ -7819,16 +7836,16 @@
       <c r="E78" s="0" t="s">
         <v>467</v>
       </c>
-      <c r="F78" s="1" t="s">
+      <c r="F78" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="G78" s="0" t="n">
+      <c r="G78" s="1" t="n">
         <v>1.9275641</v>
       </c>
-      <c r="H78" s="0" t="n">
+      <c r="H78" s="1" t="n">
         <v>0.5764837</v>
       </c>
-      <c r="I78" s="0" t="n">
+      <c r="I78" s="1" t="n">
         <v>0.11131275</v>
       </c>
     </row>
@@ -7851,13 +7868,13 @@
       <c r="F79" s="0" t="s">
         <v>473</v>
       </c>
-      <c r="G79" s="0" t="n">
+      <c r="G79" s="1" t="n">
         <v>5.697386</v>
       </c>
-      <c r="H79" s="0" t="n">
+      <c r="H79" s="1" t="n">
         <v>1.927125</v>
       </c>
-      <c r="I79" s="0" t="n">
+      <c r="I79" s="1" t="n">
         <v>0.09131718</v>
       </c>
     </row>
@@ -7880,13 +7897,13 @@
       <c r="F80" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="G80" s="0" t="n">
+      <c r="G80" s="1" t="n">
         <v>5.691096</v>
       </c>
-      <c r="H80" s="0" t="n">
+      <c r="H80" s="1" t="n">
         <v>3.2701564</v>
       </c>
-      <c r="I80" s="0" t="n">
+      <c r="I80" s="1" t="n">
         <v>0.097661376</v>
       </c>
     </row>
@@ -7909,13 +7926,13 @@
       <c r="F81" s="0" t="s">
         <v>482</v>
       </c>
-      <c r="G81" s="0" t="n">
+      <c r="G81" s="1" t="n">
         <v>5.698632</v>
       </c>
-      <c r="H81" s="0" t="n">
+      <c r="H81" s="1" t="n">
         <v>4.4865994</v>
       </c>
-      <c r="I81" s="0" t="n">
+      <c r="I81" s="1" t="n">
         <v>0.11889398</v>
       </c>
     </row>
@@ -7929,7 +7946,7 @@
       <c r="C82" s="0" t="s">
         <v>485</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="D82" s="2" t="s">
         <v>486</v>
       </c>
       <c r="E82" s="0" t="s">
@@ -7938,13 +7955,13 @@
       <c r="F82" s="0" t="s">
         <v>488</v>
       </c>
-      <c r="G82" s="0" t="n">
+      <c r="G82" s="1" t="n">
         <v>2.3203206</v>
       </c>
-      <c r="H82" s="0" t="n">
+      <c r="H82" s="1" t="n">
         <v>0.8493414</v>
       </c>
-      <c r="I82" s="0" t="n">
+      <c r="I82" s="1" t="n">
         <v>0.09945786</v>
       </c>
     </row>
@@ -7964,16 +7981,16 @@
       <c r="E83" s="0" t="s">
         <v>493</v>
       </c>
-      <c r="F83" s="1" t="s">
+      <c r="F83" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="G83" s="0" t="n">
+      <c r="G83" s="1" t="n">
         <v>0.120903015</v>
       </c>
-      <c r="H83" s="0" t="n">
+      <c r="H83" s="1" t="n">
         <v>0.6275053</v>
       </c>
-      <c r="I83" s="0" t="n">
+      <c r="I83" s="1" t="n">
         <v>0.14434636</v>
       </c>
     </row>
@@ -7996,13 +8013,13 @@
       <c r="F84" s="0" t="s">
         <v>500</v>
       </c>
-      <c r="G84" s="0" t="n">
+      <c r="G84" s="1" t="n">
         <v>4.9044347</v>
       </c>
-      <c r="H84" s="0" t="n">
+      <c r="H84" s="1" t="n">
         <v>0.43640327</v>
       </c>
-      <c r="I84" s="0" t="n">
+      <c r="I84" s="1" t="n">
         <v>0.23628485</v>
       </c>
     </row>
@@ -8025,13 +8042,13 @@
       <c r="F85" s="0" t="s">
         <v>506</v>
       </c>
-      <c r="G85" s="0" t="n">
+      <c r="G85" s="1" t="n">
         <v>0.2614684</v>
       </c>
-      <c r="H85" s="0" t="n">
+      <c r="H85" s="1" t="n">
         <v>1.6082134</v>
       </c>
-      <c r="I85" s="0" t="n">
+      <c r="I85" s="1" t="n">
         <v>0.47557223</v>
       </c>
     </row>
@@ -8054,13 +8071,13 @@
       <c r="F86" s="0" t="s">
         <v>511</v>
       </c>
-      <c r="G86" s="0" t="n">
+      <c r="G86" s="1" t="n">
         <v>5.580124</v>
       </c>
-      <c r="H86" s="0" t="n">
+      <c r="H86" s="1" t="n">
         <v>1.7004929</v>
       </c>
-      <c r="I86" s="0" t="n">
+      <c r="I86" s="1" t="n">
         <v>0.040940166</v>
       </c>
     </row>
@@ -8083,13 +8100,13 @@
       <c r="F87" s="0" t="s">
         <v>517</v>
       </c>
-      <c r="G87" s="0" t="n">
+      <c r="G87" s="1" t="n">
         <v>1.6961126</v>
       </c>
-      <c r="H87" s="0" t="n">
+      <c r="H87" s="1" t="n">
         <v>0.21253967</v>
       </c>
-      <c r="I87" s="0" t="n">
+      <c r="I87" s="1" t="n">
         <v>0.15135944</v>
       </c>
     </row>
@@ -8112,13 +8129,13 @@
       <c r="F88" s="0" t="s">
         <v>523</v>
       </c>
-      <c r="G88" s="0" t="n">
+      <c r="G88" s="1" t="n">
         <v>2.5749073</v>
       </c>
-      <c r="H88" s="0" t="n">
+      <c r="H88" s="1" t="n">
         <v>5.7199535</v>
       </c>
-      <c r="I88" s="0" t="n">
+      <c r="I88" s="1" t="n">
         <v>0.39362013</v>
       </c>
     </row>
@@ -8141,13 +8158,13 @@
       <c r="F89" s="0" t="s">
         <v>529</v>
       </c>
-      <c r="G89" s="0" t="n">
+      <c r="G89" s="1" t="n">
         <v>3.3501735</v>
       </c>
-      <c r="H89" s="0" t="n">
+      <c r="H89" s="1" t="n">
         <v>2.2358408</v>
       </c>
-      <c r="I89" s="0" t="n">
+      <c r="I89" s="1" t="n">
         <v>0.2709235</v>
       </c>
     </row>
@@ -8170,13 +8187,13 @@
       <c r="F90" s="0" t="s">
         <v>535</v>
       </c>
-      <c r="G90" s="0" t="n">
+      <c r="G90" s="1" t="n">
         <v>0.38085175</v>
       </c>
-      <c r="H90" s="0" t="n">
+      <c r="H90" s="1" t="n">
         <v>1.0060635</v>
       </c>
-      <c r="I90" s="0" t="n">
+      <c r="I90" s="1" t="n">
         <v>0.07841408</v>
       </c>
     </row>
@@ -8199,13 +8216,13 @@
       <c r="F91" s="0" t="s">
         <v>541</v>
       </c>
-      <c r="G91" s="0" t="n">
+      <c r="G91" s="1" t="n">
         <v>4.857636</v>
       </c>
-      <c r="H91" s="0" t="n">
+      <c r="H91" s="1" t="n">
         <v>0.42486286</v>
       </c>
-      <c r="I91" s="0" t="n">
+      <c r="I91" s="1" t="n">
         <v>0.07998264</v>
       </c>
     </row>
@@ -8228,13 +8245,13 @@
       <c r="F92" s="0" t="s">
         <v>547</v>
       </c>
-      <c r="G92" s="0" t="n">
+      <c r="G92" s="1" t="n">
         <v>1.9744949</v>
       </c>
-      <c r="H92" s="0" t="n">
+      <c r="H92" s="1" t="n">
         <v>4.606145</v>
       </c>
-      <c r="I92" s="0" t="n">
+      <c r="I92" s="1" t="n">
         <v>0.13626885</v>
       </c>
     </row>
@@ -8257,13 +8274,13 @@
       <c r="F93" s="0" t="s">
         <v>553</v>
       </c>
-      <c r="G93" s="0" t="n">
+      <c r="G93" s="1" t="n">
         <v>0.63125277</v>
       </c>
-      <c r="H93" s="0" t="n">
+      <c r="H93" s="1" t="n">
         <v>4.5303597</v>
       </c>
-      <c r="I93" s="0" t="n">
+      <c r="I93" s="1" t="n">
         <v>0.14437294</v>
       </c>
     </row>
@@ -8286,13 +8303,13 @@
       <c r="F94" s="0" t="s">
         <v>559</v>
       </c>
-      <c r="G94" s="0" t="n">
+      <c r="G94" s="1" t="n">
         <v>4.000094</v>
       </c>
-      <c r="H94" s="0" t="n">
+      <c r="H94" s="1" t="n">
         <v>4.7742825</v>
       </c>
-      <c r="I94" s="0" t="n">
+      <c r="I94" s="1" t="n">
         <v>0.2065413</v>
       </c>
     </row>
@@ -8315,13 +8332,13 @@
       <c r="F95" s="0" t="s">
         <v>565</v>
       </c>
-      <c r="G95" s="0" t="n">
+      <c r="G95" s="1" t="n">
         <v>2.119151</v>
       </c>
-      <c r="H95" s="0" t="n">
+      <c r="H95" s="1" t="n">
         <v>6.6143084</v>
       </c>
-      <c r="I95" s="0" t="n">
+      <c r="I95" s="1" t="n">
         <v>0.21839225</v>
       </c>
     </row>
@@ -8344,13 +8361,13 @@
       <c r="F96" s="0" t="s">
         <v>571</v>
       </c>
-      <c r="G96" s="0" t="n">
+      <c r="G96" s="1" t="n">
         <v>3.0310726</v>
       </c>
-      <c r="H96" s="0" t="n">
+      <c r="H96" s="1" t="n">
         <v>4.9129124</v>
       </c>
-      <c r="I96" s="0" t="n">
+      <c r="I96" s="1" t="n">
         <v>0.16866267</v>
       </c>
     </row>
@@ -8373,13 +8390,13 @@
       <c r="F97" s="0" t="s">
         <v>576</v>
       </c>
-      <c r="G97" s="0" t="n">
+      <c r="G97" s="1" t="n">
         <v>5.805053</v>
       </c>
-      <c r="H97" s="0" t="n">
+      <c r="H97" s="1" t="n">
         <v>2.405798</v>
       </c>
-      <c r="I97" s="0" t="n">
+      <c r="I97" s="1" t="n">
         <v>0.16550374</v>
       </c>
     </row>
@@ -8402,13 +8419,13 @@
       <c r="F98" s="0" t="s">
         <v>582</v>
       </c>
-      <c r="G98" s="0" t="n">
+      <c r="G98" s="1" t="n">
         <v>1.9675691</v>
       </c>
-      <c r="H98" s="0" t="n">
+      <c r="H98" s="1" t="n">
         <v>0.3179493</v>
       </c>
-      <c r="I98" s="0" t="n">
+      <c r="I98" s="1" t="n">
         <v>0.1273309</v>
       </c>
     </row>
@@ -8431,13 +8448,13 @@
       <c r="F99" s="0" t="s">
         <v>588</v>
       </c>
-      <c r="G99" s="0" t="n">
+      <c r="G99" s="1" t="n">
         <v>0.64379215</v>
       </c>
-      <c r="H99" s="0" t="n">
+      <c r="H99" s="1" t="n">
         <v>4.15279</v>
       </c>
-      <c r="I99" s="0" t="n">
+      <c r="I99" s="1" t="n">
         <v>0.20051658</v>
       </c>
     </row>
@@ -8460,13 +8477,13 @@
       <c r="F100" s="0" t="s">
         <v>594</v>
       </c>
-      <c r="G100" s="0" t="n">
+      <c r="G100" s="1" t="n">
         <v>5.6952643</v>
       </c>
-      <c r="H100" s="0" t="n">
+      <c r="H100" s="1" t="n">
         <v>3.3863802</v>
       </c>
-      <c r="I100" s="0" t="n">
+      <c r="I100" s="1" t="n">
         <v>0.32081628</v>
       </c>
     </row>
@@ -8489,13 +8506,13 @@
       <c r="F101" s="0" t="s">
         <v>600</v>
       </c>
-      <c r="G101" s="0" t="n">
+      <c r="G101" s="1" t="n">
         <v>2.9943643</v>
       </c>
-      <c r="H101" s="0" t="n">
+      <c r="H101" s="1" t="n">
         <v>3.9542065</v>
       </c>
-      <c r="I101" s="0" t="n">
+      <c r="I101" s="1" t="n">
         <v>0.29840946</v>
       </c>
     </row>
@@ -8509,7 +8526,7 @@
       <c r="C102" s="0" t="s">
         <v>603</v>
       </c>
-      <c r="D102" s="1" t="s">
+      <c r="D102" s="2" t="s">
         <v>604</v>
       </c>
       <c r="E102" s="0" t="s">
@@ -8518,13 +8535,13 @@
       <c r="F102" s="0" t="s">
         <v>606</v>
       </c>
-      <c r="G102" s="0" t="n">
+      <c r="G102" s="1" t="n">
         <v>4.199664</v>
       </c>
-      <c r="H102" s="0" t="n">
+      <c r="H102" s="1" t="n">
         <v>0.88660526</v>
       </c>
-      <c r="I102" s="0" t="n">
+      <c r="I102" s="1" t="n">
         <v>0.31438708</v>
       </c>
     </row>
@@ -8547,13 +8564,13 @@
       <c r="F103" s="0" t="s">
         <v>611</v>
       </c>
-      <c r="G103" s="0" t="n">
+      <c r="G103" s="1" t="n">
         <v>5.901276</v>
       </c>
-      <c r="H103" s="0" t="n">
+      <c r="H103" s="1" t="n">
         <v>0.5924969</v>
       </c>
-      <c r="I103" s="0" t="n">
+      <c r="I103" s="1" t="n">
         <v>0.35466933</v>
       </c>
     </row>
@@ -8576,13 +8593,13 @@
       <c r="F104" s="0" t="s">
         <v>617</v>
       </c>
-      <c r="G104" s="0" t="n">
+      <c r="G104" s="1" t="n">
         <v>2.9740634</v>
       </c>
-      <c r="H104" s="0" t="n">
+      <c r="H104" s="1" t="n">
         <v>2.543891</v>
       </c>
-      <c r="I104" s="0" t="n">
+      <c r="I104" s="1" t="n">
         <v>0.11539185</v>
       </c>
     </row>
@@ -8605,13 +8622,13 @@
       <c r="F105" s="0" t="s">
         <v>623</v>
       </c>
-      <c r="G105" s="0" t="n">
+      <c r="G105" s="1" t="n">
         <v>2.5175056</v>
       </c>
-      <c r="H105" s="0" t="n">
+      <c r="H105" s="1" t="n">
         <v>3.027114</v>
       </c>
-      <c r="I105" s="0" t="n">
+      <c r="I105" s="1" t="n">
         <v>0.1975435</v>
       </c>
     </row>
@@ -8634,13 +8651,13 @@
       <c r="F106" s="0" t="s">
         <v>629</v>
       </c>
-      <c r="G106" s="0" t="n">
+      <c r="G106" s="1" t="n">
         <v>1.4424319</v>
       </c>
-      <c r="H106" s="0" t="n">
+      <c r="H106" s="1" t="n">
         <v>5.3321977</v>
       </c>
-      <c r="I106" s="0" t="n">
+      <c r="I106" s="1" t="n">
         <v>0.176103</v>
       </c>
     </row>
@@ -8663,13 +8680,13 @@
       <c r="F107" s="0" t="s">
         <v>635</v>
       </c>
-      <c r="G107" s="0" t="n">
+      <c r="G107" s="1" t="n">
         <v>2.6220078</v>
       </c>
-      <c r="H107" s="0" t="n">
+      <c r="H107" s="1" t="n">
         <v>0.6260843</v>
       </c>
-      <c r="I107" s="0" t="n">
+      <c r="I107" s="1" t="n">
         <v>0.20064163</v>
       </c>
     </row>
@@ -8692,13 +8709,13 @@
       <c r="F108" s="0" t="s">
         <v>641</v>
       </c>
-      <c r="G108" s="0" t="n">
+      <c r="G108" s="1" t="n">
         <v>3.5023623</v>
       </c>
-      <c r="H108" s="0" t="n">
+      <c r="H108" s="1" t="n">
         <v>0.48252678</v>
       </c>
-      <c r="I108" s="0" t="n">
+      <c r="I108" s="1" t="n">
         <v>0.21501589</v>
       </c>
     </row>
@@ -8721,13 +8738,13 @@
       <c r="F109" s="0" t="s">
         <v>647</v>
       </c>
-      <c r="G109" s="0" t="n">
+      <c r="G109" s="1" t="n">
         <v>4.5864587</v>
       </c>
-      <c r="H109" s="0" t="n">
+      <c r="H109" s="1" t="n">
         <v>0.30072594</v>
       </c>
-      <c r="I109" s="0" t="n">
+      <c r="I109" s="1" t="n">
         <v>0.18129599</v>
       </c>
     </row>
@@ -8750,13 +8767,13 @@
       <c r="F110" s="0" t="s">
         <v>653</v>
       </c>
-      <c r="G110" s="0" t="n">
+      <c r="G110" s="1" t="n">
         <v>1.422256</v>
       </c>
-      <c r="H110" s="0" t="n">
+      <c r="H110" s="1" t="n">
         <v>4.7829695</v>
       </c>
-      <c r="I110" s="0" t="n">
+      <c r="I110" s="1" t="n">
         <v>0.20989871</v>
       </c>
     </row>
@@ -8779,13 +8796,13 @@
       <c r="F111" s="0" t="s">
         <v>659</v>
       </c>
-      <c r="G111" s="0" t="n">
+      <c r="G111" s="1" t="n">
         <v>0.20491648</v>
       </c>
-      <c r="H111" s="0" t="n">
+      <c r="H111" s="1" t="n">
         <v>4.0088625</v>
       </c>
-      <c r="I111" s="0" t="n">
+      <c r="I111" s="1" t="n">
         <v>0.2742008</v>
       </c>
     </row>
@@ -8808,13 +8825,13 @@
       <c r="F112" s="0" t="s">
         <v>665</v>
       </c>
-      <c r="G112" s="0" t="n">
+      <c r="G112" s="1" t="n">
         <v>0.14249468</v>
       </c>
-      <c r="H112" s="0" t="n">
+      <c r="H112" s="1" t="n">
         <v>0.6145754</v>
       </c>
-      <c r="I112" s="0" t="n">
+      <c r="I112" s="1" t="n">
         <v>0.27764988</v>
       </c>
     </row>
@@ -8837,13 +8854,13 @@
       <c r="F113" s="0" t="s">
         <v>671</v>
       </c>
-      <c r="G113" s="0" t="n">
+      <c r="G113" s="1" t="n">
         <v>4.669228</v>
       </c>
-      <c r="H113" s="0" t="n">
+      <c r="H113" s="1" t="n">
         <v>0.97824574</v>
       </c>
-      <c r="I113" s="0" t="n">
+      <c r="I113" s="1" t="n">
         <v>0.22322583</v>
       </c>
     </row>
@@ -8866,13 +8883,13 @@
       <c r="F114" s="0" t="s">
         <v>677</v>
       </c>
-      <c r="G114" s="0" t="n">
+      <c r="G114" s="1" t="n">
         <v>4.614986</v>
       </c>
-      <c r="H114" s="0" t="n">
+      <c r="H114" s="1" t="n">
         <v>7.0210433</v>
       </c>
-      <c r="I114" s="0" t="n">
+      <c r="I114" s="1" t="n">
         <v>0.27628934</v>
       </c>
     </row>
@@ -8895,13 +8912,13 @@
       <c r="F115" s="0" t="s">
         <v>683</v>
       </c>
-      <c r="G115" s="0" t="n">
+      <c r="G115" s="1" t="n">
         <v>0.24186039</v>
       </c>
-      <c r="H115" s="0" t="n">
+      <c r="H115" s="1" t="n">
         <v>0.020300865</v>
       </c>
-      <c r="I115" s="0" t="n">
+      <c r="I115" s="1" t="n">
         <v>0.17688227</v>
       </c>
     </row>
@@ -8924,13 +8941,13 @@
       <c r="F116" s="0" t="s">
         <v>689</v>
       </c>
-      <c r="G116" s="0" t="n">
+      <c r="G116" s="1" t="n">
         <v>2.2525063</v>
       </c>
-      <c r="H116" s="0" t="n">
+      <c r="H116" s="1" t="n">
         <v>1.1572094</v>
       </c>
-      <c r="I116" s="0" t="n">
+      <c r="I116" s="1" t="n">
         <v>0.1732117</v>
       </c>
     </row>
@@ -8953,13 +8970,13 @@
       <c r="F117" s="0" t="s">
         <v>695</v>
       </c>
-      <c r="G117" s="0" t="n">
+      <c r="G117" s="1" t="n">
         <v>0.40184736</v>
       </c>
-      <c r="H117" s="0" t="n">
+      <c r="H117" s="1" t="n">
         <v>2.4523125</v>
       </c>
-      <c r="I117" s="0" t="n">
+      <c r="I117" s="1" t="n">
         <v>0.15690994</v>
       </c>
     </row>
@@ -8982,13 +8999,13 @@
       <c r="F118" s="0" t="s">
         <v>701</v>
       </c>
-      <c r="G118" s="0" t="n">
+      <c r="G118" s="1" t="n">
         <v>2.243878</v>
       </c>
-      <c r="H118" s="0" t="n">
+      <c r="H118" s="1" t="n">
         <v>3.2661219</v>
       </c>
-      <c r="I118" s="0" t="n">
+      <c r="I118" s="1" t="n">
         <v>0.12872374</v>
       </c>
     </row>
@@ -9011,13 +9028,13 @@
       <c r="F119" s="0" t="s">
         <v>707</v>
       </c>
-      <c r="G119" s="0" t="n">
+      <c r="G119" s="1" t="n">
         <v>5.6921015</v>
       </c>
-      <c r="H119" s="0" t="n">
+      <c r="H119" s="1" t="n">
         <v>2.7074747</v>
       </c>
-      <c r="I119" s="0" t="n">
+      <c r="I119" s="1" t="n">
         <v>0.12095368</v>
       </c>
     </row>
@@ -9034,19 +9051,19 @@
       <c r="D120" s="0" t="s">
         <v>711</v>
       </c>
-      <c r="E120" s="1" t="s">
+      <c r="E120" s="2" t="s">
         <v>712</v>
       </c>
-      <c r="F120" s="1" t="s">
+      <c r="F120" s="2" t="s">
         <v>713</v>
       </c>
-      <c r="G120" s="0" t="n">
+      <c r="G120" s="1" t="n">
         <v>7.699067</v>
       </c>
-      <c r="H120" s="0" t="n">
+      <c r="H120" s="1" t="n">
         <v>4.571761</v>
       </c>
-      <c r="I120" s="0" t="n">
+      <c r="I120" s="1" t="n">
         <v>0.13164556</v>
       </c>
     </row>
@@ -9063,19 +9080,19 @@
       <c r="D121" s="0" t="s">
         <v>717</v>
       </c>
-      <c r="E121" s="1" t="s">
+      <c r="E121" s="2" t="s">
         <v>718</v>
       </c>
       <c r="F121" s="0" t="s">
         <v>719</v>
       </c>
-      <c r="G121" s="0" t="n">
+      <c r="G121" s="1" t="n">
         <v>4.375318</v>
       </c>
-      <c r="H121" s="0" t="n">
+      <c r="H121" s="1" t="n">
         <v>0.8815422</v>
       </c>
-      <c r="I121" s="0" t="n">
+      <c r="I121" s="1" t="n">
         <v>0.13199961</v>
       </c>
     </row>
@@ -9092,19 +9109,19 @@
       <c r="D122" s="0" t="s">
         <v>723</v>
       </c>
-      <c r="E122" s="1" t="s">
+      <c r="E122" s="2" t="s">
         <v>724</v>
       </c>
-      <c r="F122" s="1" t="s">
+      <c r="F122" s="2" t="s">
         <v>725</v>
       </c>
-      <c r="G122" s="0" t="n">
+      <c r="G122" s="1" t="n">
         <v>1.0155516</v>
       </c>
-      <c r="H122" s="0" t="n">
+      <c r="H122" s="1" t="n">
         <v>2.9088945</v>
       </c>
-      <c r="I122" s="0" t="n">
+      <c r="I122" s="1" t="n">
         <v>0.072618484</v>
       </c>
     </row>
@@ -9124,16 +9141,16 @@
       <c r="E123" s="0" t="s">
         <v>730</v>
       </c>
-      <c r="F123" s="1" t="s">
+      <c r="F123" s="2" t="s">
         <v>725</v>
       </c>
-      <c r="G123" s="0" t="n">
+      <c r="G123" s="1" t="n">
         <v>3.8976202</v>
       </c>
-      <c r="H123" s="0" t="n">
+      <c r="H123" s="1" t="n">
         <v>2.0886536</v>
       </c>
-      <c r="I123" s="0" t="n">
+      <c r="I123" s="1" t="n">
         <v>0.13809192</v>
       </c>
     </row>
@@ -9150,19 +9167,19 @@
       <c r="D124" s="0" t="s">
         <v>734</v>
       </c>
-      <c r="E124" s="1" t="s">
+      <c r="E124" s="2" t="s">
         <v>735</v>
       </c>
       <c r="F124" s="0" t="s">
         <v>736</v>
       </c>
-      <c r="G124" s="0" t="n">
+      <c r="G124" s="1" t="n">
         <v>0.97449875</v>
       </c>
-      <c r="H124" s="0" t="n">
+      <c r="H124" s="1" t="n">
         <v>1.5214462</v>
       </c>
-      <c r="I124" s="0" t="n">
+      <c r="I124" s="1" t="n">
         <v>0.10202646</v>
       </c>
     </row>
@@ -9185,13 +9202,13 @@
       <c r="F125" s="0" t="s">
         <v>742</v>
       </c>
-      <c r="G125" s="0" t="n">
+      <c r="G125" s="1" t="n">
         <v>4.5410748</v>
       </c>
-      <c r="H125" s="0" t="n">
+      <c r="H125" s="1" t="n">
         <v>3.8471174</v>
       </c>
-      <c r="I125" s="0" t="n">
+      <c r="I125" s="1" t="n">
         <v>0.09479308</v>
       </c>
     </row>
@@ -9214,13 +9231,13 @@
       <c r="F126" s="0" t="s">
         <v>748</v>
       </c>
-      <c r="G126" s="0" t="n">
+      <c r="G126" s="1" t="n">
         <v>1.3105965</v>
       </c>
-      <c r="H126" s="0" t="n">
+      <c r="H126" s="1" t="n">
         <v>0.70563984</v>
       </c>
-      <c r="I126" s="0" t="n">
+      <c r="I126" s="1" t="n">
         <v>0.10491979</v>
       </c>
     </row>
@@ -9243,13 +9260,13 @@
       <c r="F127" s="0" t="s">
         <v>754</v>
       </c>
-      <c r="G127" s="0" t="n">
+      <c r="G127" s="1" t="n">
         <v>0.74667835</v>
       </c>
-      <c r="H127" s="0" t="n">
+      <c r="H127" s="1" t="n">
         <v>0.21643925</v>
       </c>
-      <c r="I127" s="0" t="n">
+      <c r="I127" s="1" t="n">
         <v>0.11711669</v>
       </c>
     </row>
@@ -9272,13 +9289,13 @@
       <c r="F128" s="0" t="s">
         <v>760</v>
       </c>
-      <c r="G128" s="0" t="n">
+      <c r="G128" s="1" t="n">
         <v>0.9256449</v>
       </c>
-      <c r="H128" s="0" t="n">
+      <c r="H128" s="1" t="n">
         <v>2.7565804</v>
       </c>
-      <c r="I128" s="0" t="n">
+      <c r="I128" s="1" t="n">
         <v>0.073581815</v>
       </c>
     </row>
@@ -9301,13 +9318,13 @@
       <c r="F129" s="0" t="s">
         <v>766</v>
       </c>
-      <c r="G129" s="0" t="n">
+      <c r="G129" s="1" t="n">
         <v>1.264719</v>
       </c>
-      <c r="H129" s="0" t="n">
+      <c r="H129" s="1" t="n">
         <v>0.30270767</v>
       </c>
-      <c r="I129" s="0" t="n">
+      <c r="I129" s="1" t="n">
         <v>0.113981605</v>
       </c>
     </row>
@@ -9327,16 +9344,16 @@
       <c r="E130" s="0" t="s">
         <v>771</v>
       </c>
-      <c r="F130" s="1" t="s">
+      <c r="F130" s="2" t="s">
         <v>772</v>
       </c>
-      <c r="G130" s="0" t="n">
+      <c r="G130" s="1" t="n">
         <v>0.8114824</v>
       </c>
-      <c r="H130" s="0" t="n">
+      <c r="H130" s="1" t="n">
         <v>0.95175266</v>
       </c>
-      <c r="I130" s="0" t="n">
+      <c r="I130" s="1" t="n">
         <v>0.066462636</v>
       </c>
     </row>
@@ -9353,19 +9370,19 @@
       <c r="D131" s="0" t="s">
         <v>776</v>
       </c>
-      <c r="E131" s="1" t="s">
+      <c r="E131" s="2" t="s">
         <v>777</v>
       </c>
       <c r="F131" s="0" t="s">
         <v>778</v>
       </c>
-      <c r="G131" s="0" t="n">
+      <c r="G131" s="1" t="n">
         <v>3.0386486</v>
       </c>
-      <c r="H131" s="0" t="n">
+      <c r="H131" s="1" t="n">
         <v>2.149022</v>
       </c>
-      <c r="I131" s="0" t="n">
+      <c r="I131" s="1" t="n">
         <v>0.10950458</v>
       </c>
     </row>
@@ -9388,13 +9405,13 @@
       <c r="F132" s="0" t="s">
         <v>784</v>
       </c>
-      <c r="G132" s="0" t="n">
+      <c r="G132" s="1" t="n">
         <v>1.8553753</v>
       </c>
-      <c r="H132" s="0" t="n">
+      <c r="H132" s="1" t="n">
         <v>5.0876226</v>
       </c>
-      <c r="I132" s="0" t="n">
+      <c r="I132" s="1" t="n">
         <v>0.06793368</v>
       </c>
     </row>
@@ -9414,16 +9431,16 @@
       <c r="E133" s="0" t="s">
         <v>789</v>
       </c>
-      <c r="F133" s="1" t="s">
+      <c r="F133" s="2" t="s">
         <v>790</v>
       </c>
-      <c r="G133" s="0" t="n">
+      <c r="G133" s="1" t="n">
         <v>6.4988866</v>
       </c>
-      <c r="H133" s="0" t="n">
+      <c r="H133" s="1" t="n">
         <v>8.108252</v>
       </c>
-      <c r="I133" s="0" t="n">
+      <c r="I133" s="1" t="n">
         <v>0.07750368</v>
       </c>
     </row>
@@ -9446,13 +9463,13 @@
       <c r="F134" s="0" t="s">
         <v>796</v>
       </c>
-      <c r="G134" s="0" t="n">
+      <c r="G134" s="1" t="n">
         <v>6.1500654</v>
       </c>
-      <c r="H134" s="0" t="n">
+      <c r="H134" s="1" t="n">
         <v>4.623518</v>
       </c>
-      <c r="I134" s="0" t="n">
+      <c r="I134" s="1" t="n">
         <v>0.07316196</v>
       </c>
     </row>
@@ -9475,13 +9492,13 @@
       <c r="F135" s="0" t="s">
         <v>802</v>
       </c>
-      <c r="G135" s="0" t="n">
+      <c r="G135" s="1" t="n">
         <v>7.3879447</v>
       </c>
-      <c r="H135" s="0" t="n">
+      <c r="H135" s="1" t="n">
         <v>5.6032343</v>
       </c>
-      <c r="I135" s="0" t="n">
+      <c r="I135" s="1" t="n">
         <v>0.055143833</v>
       </c>
     </row>
@@ -9504,13 +9521,13 @@
       <c r="F136" s="0" t="s">
         <v>808</v>
       </c>
-      <c r="G136" s="0" t="n">
+      <c r="G136" s="1" t="n">
         <v>2.6325045</v>
       </c>
-      <c r="H136" s="0" t="n">
+      <c r="H136" s="1" t="n">
         <v>3.29327</v>
       </c>
-      <c r="I136" s="0" t="n">
+      <c r="I136" s="1" t="n">
         <v>0.08826673</v>
       </c>
     </row>
@@ -9533,13 +9550,13 @@
       <c r="F137" s="0" t="s">
         <v>814</v>
       </c>
-      <c r="G137" s="0" t="n">
+      <c r="G137" s="1" t="n">
         <v>1.4315643</v>
       </c>
-      <c r="H137" s="0" t="n">
+      <c r="H137" s="1" t="n">
         <v>4.357193</v>
       </c>
-      <c r="I137" s="0" t="n">
+      <c r="I137" s="1" t="n">
         <v>0.1193825</v>
       </c>
     </row>
@@ -9562,13 +9579,13 @@
       <c r="F138" s="0" t="s">
         <v>820</v>
       </c>
-      <c r="G138" s="0" t="n">
+      <c r="G138" s="1" t="n">
         <v>2.7448997</v>
       </c>
-      <c r="H138" s="0" t="n">
+      <c r="H138" s="1" t="n">
         <v>0.80189514</v>
       </c>
-      <c r="I138" s="0" t="n">
+      <c r="I138" s="1" t="n">
         <v>0.17742264</v>
       </c>
     </row>
@@ -9591,13 +9608,13 @@
       <c r="F139" s="0" t="s">
         <v>826</v>
       </c>
-      <c r="G139" s="0" t="n">
+      <c r="G139" s="1" t="n">
         <v>1.5479527</v>
       </c>
-      <c r="H139" s="0" t="n">
+      <c r="H139" s="1" t="n">
         <v>4.4599676</v>
       </c>
-      <c r="I139" s="0" t="n">
+      <c r="I139" s="1" t="n">
         <v>0.08605993</v>
       </c>
     </row>
@@ -9620,13 +9637,13 @@
       <c r="F140" s="0" t="s">
         <v>832</v>
       </c>
-      <c r="G140" s="0" t="n">
+      <c r="G140" s="1" t="n">
         <v>4.823165</v>
       </c>
-      <c r="H140" s="0" t="n">
+      <c r="H140" s="1" t="n">
         <v>6.571661</v>
       </c>
-      <c r="I140" s="0" t="n">
+      <c r="I140" s="1" t="n">
         <v>0.15873158</v>
       </c>
     </row>
@@ -9649,13 +9666,13 @@
       <c r="F141" s="0" t="s">
         <v>838</v>
       </c>
-      <c r="G141" s="0" t="n">
+      <c r="G141" s="1" t="n">
         <v>0.70984936</v>
       </c>
-      <c r="H141" s="0" t="n">
+      <c r="H141" s="1" t="n">
         <v>1.1457224</v>
       </c>
-      <c r="I141" s="0" t="n">
+      <c r="I141" s="1" t="n">
         <v>0.102561235</v>
       </c>
     </row>
@@ -9678,13 +9695,13 @@
       <c r="F142" s="0" t="s">
         <v>844</v>
       </c>
-      <c r="G142" s="0" t="n">
+      <c r="G142" s="1" t="n">
         <v>1.2549305</v>
       </c>
-      <c r="H142" s="0" t="n">
+      <c r="H142" s="1" t="n">
         <v>4.3838587</v>
       </c>
-      <c r="I142" s="0" t="n">
+      <c r="I142" s="1" t="n">
         <v>0.15950382</v>
       </c>
     </row>
@@ -9707,13 +9724,13 @@
       <c r="F143" s="0" t="s">
         <v>850</v>
       </c>
-      <c r="G143" s="0" t="n">
+      <c r="G143" s="1" t="n">
         <v>0.9646988</v>
       </c>
-      <c r="H143" s="0" t="n">
+      <c r="H143" s="1" t="n">
         <v>5.858897</v>
       </c>
-      <c r="I143" s="0" t="n">
+      <c r="I143" s="1" t="n">
         <v>0.056299925</v>
       </c>
     </row>
@@ -9736,13 +9753,13 @@
       <c r="F144" s="0" t="s">
         <v>856</v>
       </c>
-      <c r="G144" s="0" t="n">
+      <c r="G144" s="1" t="n">
         <v>0.82751274</v>
       </c>
-      <c r="H144" s="0" t="n">
+      <c r="H144" s="1" t="n">
         <v>0.124619484</v>
       </c>
-      <c r="I144" s="0" t="n">
+      <c r="I144" s="1" t="n">
         <v>0.107106805</v>
       </c>
     </row>
@@ -9765,13 +9782,13 @@
       <c r="F145" s="0" t="s">
         <v>862</v>
       </c>
-      <c r="G145" s="0" t="n">
+      <c r="G145" s="1" t="n">
         <v>5.947255</v>
       </c>
-      <c r="H145" s="0" t="n">
+      <c r="H145" s="1" t="n">
         <v>1.0218029</v>
       </c>
-      <c r="I145" s="0" t="n">
+      <c r="I145" s="1" t="n">
         <v>0.07465315</v>
       </c>
     </row>
@@ -9794,13 +9811,13 @@
       <c r="F146" s="0" t="s">
         <v>868</v>
       </c>
-      <c r="G146" s="0" t="n">
+      <c r="G146" s="1" t="n">
         <v>1.2384605</v>
       </c>
-      <c r="H146" s="0" t="n">
+      <c r="H146" s="1" t="n">
         <v>0.6804571</v>
       </c>
-      <c r="I146" s="0" t="n">
+      <c r="I146" s="1" t="n">
         <v>0.13802624</v>
       </c>
     </row>
@@ -9823,13 +9840,13 @@
       <c r="F147" s="0" t="s">
         <v>874</v>
       </c>
-      <c r="G147" s="0" t="n">
+      <c r="G147" s="1" t="n">
         <v>3.826167</v>
       </c>
-      <c r="H147" s="0" t="n">
+      <c r="H147" s="1" t="n">
         <v>1.6156292</v>
       </c>
-      <c r="I147" s="0" t="n">
+      <c r="I147" s="1" t="n">
         <v>0.12740827</v>
       </c>
     </row>
@@ -9852,13 +9869,13 @@
       <c r="F148" s="0" t="s">
         <v>880</v>
       </c>
-      <c r="G148" s="0" t="n">
+      <c r="G148" s="1" t="n">
         <v>0.52805805</v>
       </c>
-      <c r="H148" s="0" t="n">
+      <c r="H148" s="1" t="n">
         <v>1.8269148</v>
       </c>
-      <c r="I148" s="0" t="n">
+      <c r="I148" s="1" t="n">
         <v>0.12944317</v>
       </c>
     </row>
@@ -9881,13 +9898,13 @@
       <c r="F149" s="0" t="s">
         <v>886</v>
       </c>
-      <c r="G149" s="0" t="n">
+      <c r="G149" s="1" t="n">
         <v>0.95262146</v>
       </c>
-      <c r="H149" s="0" t="n">
+      <c r="H149" s="1" t="n">
         <v>0.59623337</v>
       </c>
-      <c r="I149" s="0" t="n">
+      <c r="I149" s="1" t="n">
         <v>0.15818381</v>
       </c>
     </row>
@@ -9910,13 +9927,13 @@
       <c r="F150" s="0" t="s">
         <v>892</v>
       </c>
-      <c r="G150" s="0" t="n">
+      <c r="G150" s="1" t="n">
         <v>5.1968784</v>
       </c>
-      <c r="H150" s="0" t="n">
+      <c r="H150" s="1" t="n">
         <v>1.3442059</v>
       </c>
-      <c r="I150" s="0" t="n">
+      <c r="I150" s="1" t="n">
         <v>0.12959385</v>
       </c>
     </row>
@@ -9939,13 +9956,13 @@
       <c r="F151" s="0" t="s">
         <v>898</v>
       </c>
-      <c r="G151" s="0" t="n">
+      <c r="G151" s="1" t="n">
         <v>2.1314735</v>
       </c>
-      <c r="H151" s="0" t="n">
+      <c r="H151" s="1" t="n">
         <v>3.3685513</v>
       </c>
-      <c r="I151" s="0" t="n">
+      <c r="I151" s="1" t="n">
         <v>0.07532966</v>
       </c>
     </row>
@@ -9968,13 +9985,13 @@
       <c r="F152" s="0" t="s">
         <v>904</v>
       </c>
-      <c r="G152" s="0" t="n">
+      <c r="G152" s="1" t="n">
         <v>1.1559334</v>
       </c>
-      <c r="H152" s="0" t="n">
+      <c r="H152" s="1" t="n">
         <v>1.8422031</v>
       </c>
-      <c r="I152" s="0" t="n">
+      <c r="I152" s="1" t="n">
         <v>0.07507992</v>
       </c>
     </row>
@@ -9997,13 +10014,13 @@
       <c r="F153" s="0" t="s">
         <v>910</v>
       </c>
-      <c r="G153" s="0" t="n">
+      <c r="G153" s="1" t="n">
         <v>1.325346</v>
       </c>
-      <c r="H153" s="0" t="n">
+      <c r="H153" s="1" t="n">
         <v>0.90986824</v>
       </c>
-      <c r="I153" s="0" t="n">
+      <c r="I153" s="1" t="n">
         <v>0.06915176</v>
       </c>
     </row>
@@ -10026,13 +10043,13 @@
       <c r="F154" s="0" t="s">
         <v>916</v>
       </c>
-      <c r="G154" s="0" t="n">
+      <c r="G154" s="1" t="n">
         <v>2.3640728</v>
       </c>
-      <c r="H154" s="0" t="n">
+      <c r="H154" s="1" t="n">
         <v>0.848052</v>
       </c>
-      <c r="I154" s="0" t="n">
+      <c r="I154" s="1" t="n">
         <v>0.053532004</v>
       </c>
     </row>
@@ -10055,13 +10072,13 @@
       <c r="F155" s="0" t="s">
         <v>922</v>
       </c>
-      <c r="G155" s="0" t="n">
+      <c r="G155" s="1" t="n">
         <v>4.9100733</v>
       </c>
-      <c r="H155" s="0" t="n">
+      <c r="H155" s="1" t="n">
         <v>0.95492935</v>
       </c>
-      <c r="I155" s="0" t="n">
+      <c r="I155" s="1" t="n">
         <v>0.07869077</v>
       </c>
     </row>
@@ -10075,7 +10092,7 @@
       <c r="C156" s="0" t="s">
         <v>925</v>
       </c>
-      <c r="D156" s="1" t="s">
+      <c r="D156" s="2" t="s">
         <v>926</v>
       </c>
       <c r="E156" s="0" t="s">
@@ -10084,13 +10101,13 @@
       <c r="F156" s="0" t="s">
         <v>928</v>
       </c>
-      <c r="G156" s="0" t="n">
+      <c r="G156" s="1" t="n">
         <v>0.8496971</v>
       </c>
-      <c r="H156" s="0" t="n">
+      <c r="H156" s="1" t="n">
         <v>1.8321095</v>
       </c>
-      <c r="I156" s="0" t="n">
+      <c r="I156" s="1" t="n">
         <v>0.091385245</v>
       </c>
     </row>
@@ -10113,13 +10130,13 @@
       <c r="F157" s="0" t="s">
         <v>934</v>
       </c>
-      <c r="G157" s="0" t="n">
+      <c r="G157" s="1" t="n">
         <v>1.9113121</v>
       </c>
-      <c r="H157" s="0" t="n">
+      <c r="H157" s="1" t="n">
         <v>0.85645866</v>
       </c>
-      <c r="I157" s="0" t="n">
+      <c r="I157" s="1" t="n">
         <v>0.086856365</v>
       </c>
     </row>
@@ -10142,13 +10159,13 @@
       <c r="F158" s="0" t="s">
         <v>940</v>
       </c>
-      <c r="G158" s="0" t="n">
+      <c r="G158" s="1" t="n">
         <v>1.3604002</v>
       </c>
-      <c r="H158" s="0" t="n">
+      <c r="H158" s="1" t="n">
         <v>2.752263</v>
       </c>
-      <c r="I158" s="0" t="n">
+      <c r="I158" s="1" t="n">
         <v>0.095850945</v>
       </c>
     </row>
@@ -10171,13 +10188,13 @@
       <c r="F159" s="0" t="s">
         <v>946</v>
       </c>
-      <c r="G159" s="0" t="n">
+      <c r="G159" s="1" t="n">
         <v>2.1537495</v>
       </c>
-      <c r="H159" s="0" t="n">
+      <c r="H159" s="1" t="n">
         <v>0.83192635</v>
       </c>
-      <c r="I159" s="0" t="n">
+      <c r="I159" s="1" t="n">
         <v>0.09770739</v>
       </c>
     </row>
@@ -10200,13 +10217,13 @@
       <c r="F160" s="0" t="s">
         <v>952</v>
       </c>
-      <c r="G160" s="0" t="n">
+      <c r="G160" s="1" t="n">
         <v>3.5612097</v>
       </c>
-      <c r="H160" s="0" t="n">
+      <c r="H160" s="1" t="n">
         <v>3.8399878</v>
       </c>
-      <c r="I160" s="0" t="n">
+      <c r="I160" s="1" t="n">
         <v>0.066545844</v>
       </c>
     </row>
@@ -10220,7 +10237,7 @@
       <c r="C161" s="0" t="s">
         <v>955</v>
       </c>
-      <c r="D161" s="1" t="s">
+      <c r="D161" s="2" t="s">
         <v>956</v>
       </c>
       <c r="E161" s="0" t="s">
@@ -10229,13 +10246,13 @@
       <c r="F161" s="0" t="s">
         <v>958</v>
       </c>
-      <c r="G161" s="0" t="n">
+      <c r="G161" s="1" t="n">
         <v>5.0984344</v>
       </c>
-      <c r="H161" s="0" t="n">
+      <c r="H161" s="1" t="n">
         <v>0.08532429</v>
       </c>
-      <c r="I161" s="0" t="n">
+      <c r="I161" s="1" t="n">
         <v>0.0879364</v>
       </c>
     </row>
@@ -10258,13 +10275,13 @@
       <c r="F162" s="0" t="s">
         <v>964</v>
       </c>
-      <c r="G162" s="0" t="n">
+      <c r="G162" s="1" t="n">
         <v>2.710679</v>
       </c>
-      <c r="H162" s="0" t="n">
+      <c r="H162" s="1" t="n">
         <v>2.5194573</v>
       </c>
-      <c r="I162" s="0" t="n">
+      <c r="I162" s="1" t="n">
         <v>0.13419366</v>
       </c>
     </row>
@@ -10287,13 +10304,13 @@
       <c r="F163" s="0" t="s">
         <v>970</v>
       </c>
-      <c r="G163" s="0" t="n">
+      <c r="G163" s="1" t="n">
         <v>0.17297268</v>
       </c>
-      <c r="H163" s="0" t="n">
+      <c r="H163" s="1" t="n">
         <v>1.7875805</v>
       </c>
-      <c r="I163" s="0" t="n">
+      <c r="I163" s="1" t="n">
         <v>0.080966234</v>
       </c>
     </row>
@@ -10316,13 +10333,13 @@
       <c r="F164" s="0" t="s">
         <v>976</v>
       </c>
-      <c r="G164" s="0" t="n">
+      <c r="G164" s="1" t="n">
         <v>4.15884</v>
       </c>
-      <c r="H164" s="0" t="n">
+      <c r="H164" s="1" t="n">
         <v>0.87337065</v>
       </c>
-      <c r="I164" s="0" t="n">
+      <c r="I164" s="1" t="n">
         <v>0.060697317</v>
       </c>
     </row>
@@ -10345,13 +10362,13 @@
       <c r="F165" s="0" t="s">
         <v>982</v>
       </c>
-      <c r="G165" s="0" t="n">
+      <c r="G165" s="1" t="n">
         <v>1.7172279</v>
       </c>
-      <c r="H165" s="0" t="n">
+      <c r="H165" s="1" t="n">
         <v>2.3729906</v>
       </c>
-      <c r="I165" s="0" t="n">
+      <c r="I165" s="1" t="n">
         <v>0.0491966</v>
       </c>
     </row>
@@ -10371,16 +10388,16 @@
       <c r="E166" s="0" t="s">
         <v>987</v>
       </c>
-      <c r="F166" s="1" t="s">
+      <c r="F166" s="2" t="s">
         <v>988</v>
       </c>
-      <c r="G166" s="0" t="n">
+      <c r="G166" s="1" t="n">
         <v>1.7402792</v>
       </c>
-      <c r="H166" s="0" t="n">
+      <c r="H166" s="1" t="n">
         <v>0.6247916</v>
       </c>
-      <c r="I166" s="0" t="n">
+      <c r="I166" s="1" t="n">
         <v>0.10881257</v>
       </c>
     </row>
@@ -10400,16 +10417,16 @@
       <c r="E167" s="0" t="s">
         <v>993</v>
       </c>
-      <c r="F167" s="1" t="s">
+      <c r="F167" s="2" t="s">
         <v>994</v>
       </c>
-      <c r="G167" s="0" t="n">
+      <c r="G167" s="1" t="n">
         <v>2.1838026</v>
       </c>
-      <c r="H167" s="0" t="n">
+      <c r="H167" s="1" t="n">
         <v>2.5995913</v>
       </c>
-      <c r="I167" s="0" t="n">
+      <c r="I167" s="1" t="n">
         <v>0.1103276</v>
       </c>
     </row>
@@ -10432,13 +10449,13 @@
       <c r="F168" s="0" t="s">
         <v>1000</v>
       </c>
-      <c r="G168" s="0" t="n">
+      <c r="G168" s="1" t="n">
         <v>0.3883648</v>
       </c>
-      <c r="H168" s="0" t="n">
+      <c r="H168" s="1" t="n">
         <v>1.9563117</v>
       </c>
-      <c r="I168" s="0" t="n">
+      <c r="I168" s="1" t="n">
         <v>0.10936725</v>
       </c>
     </row>
@@ -10461,13 +10478,13 @@
       <c r="F169" s="0" t="s">
         <v>1006</v>
       </c>
-      <c r="G169" s="0" t="n">
+      <c r="G169" s="1" t="n">
         <v>0.13171768</v>
       </c>
-      <c r="H169" s="0" t="n">
+      <c r="H169" s="1" t="n">
         <v>0.13235712</v>
       </c>
-      <c r="I169" s="0" t="n">
+      <c r="I169" s="1" t="n">
         <v>0.11642206</v>
       </c>
     </row>
@@ -10490,13 +10507,13 @@
       <c r="F170" s="0" t="s">
         <v>1012</v>
       </c>
-      <c r="G170" s="0" t="n">
+      <c r="G170" s="1" t="n">
         <v>1.3323774</v>
       </c>
-      <c r="H170" s="0" t="n">
+      <c r="H170" s="1" t="n">
         <v>1.5138302</v>
       </c>
-      <c r="I170" s="0" t="n">
+      <c r="I170" s="1" t="n">
         <v>0.1143353</v>
       </c>
     </row>
@@ -10519,13 +10536,13 @@
       <c r="F171" s="0" t="s">
         <v>1018</v>
       </c>
-      <c r="G171" s="0" t="n">
+      <c r="G171" s="1" t="n">
         <v>0.059523582</v>
       </c>
-      <c r="H171" s="0" t="n">
+      <c r="H171" s="1" t="n">
         <v>1.9401679</v>
       </c>
-      <c r="I171" s="0" t="n">
+      <c r="I171" s="1" t="n">
         <v>0.13889074</v>
       </c>
     </row>
@@ -10548,13 +10565,13 @@
       <c r="F172" s="0" t="s">
         <v>1024</v>
       </c>
-      <c r="G172" s="0" t="n">
+      <c r="G172" s="1" t="n">
         <v>5.9063253</v>
       </c>
-      <c r="H172" s="0" t="n">
+      <c r="H172" s="1" t="n">
         <v>3.1689167</v>
       </c>
-      <c r="I172" s="0" t="n">
+      <c r="I172" s="1" t="n">
         <v>0.05401635</v>
       </c>
     </row>
@@ -10577,13 +10594,13 @@
       <c r="F173" s="0" t="s">
         <v>1030</v>
       </c>
-      <c r="G173" s="0" t="n">
+      <c r="G173" s="1" t="n">
         <v>2.609231</v>
       </c>
-      <c r="H173" s="0" t="n">
+      <c r="H173" s="1" t="n">
         <v>0.616354</v>
       </c>
-      <c r="I173" s="0" t="n">
+      <c r="I173" s="1" t="n">
         <v>0.09417415</v>
       </c>
     </row>
@@ -10606,13 +10623,13 @@
       <c r="F174" s="0" t="s">
         <v>1036</v>
       </c>
-      <c r="G174" s="0" t="n">
+      <c r="G174" s="1" t="n">
         <v>5.4273596</v>
       </c>
-      <c r="H174" s="0" t="n">
+      <c r="H174" s="1" t="n">
         <v>4.5454845</v>
       </c>
-      <c r="I174" s="0" t="n">
+      <c r="I174" s="1" t="n">
         <v>0.0753243</v>
       </c>
     </row>
@@ -10635,13 +10652,13 @@
       <c r="F175" s="0" t="s">
         <v>1042</v>
       </c>
-      <c r="G175" s="0" t="n">
+      <c r="G175" s="1" t="n">
         <v>3.6181984</v>
       </c>
-      <c r="H175" s="0" t="n">
+      <c r="H175" s="1" t="n">
         <v>2.6931517</v>
       </c>
-      <c r="I175" s="0" t="n">
+      <c r="I175" s="1" t="n">
         <v>0.109681964</v>
       </c>
     </row>
@@ -10664,13 +10681,13 @@
       <c r="F176" s="0" t="s">
         <v>1048</v>
       </c>
-      <c r="G176" s="0" t="n">
+      <c r="G176" s="1" t="n">
         <v>2.2222013</v>
       </c>
-      <c r="H176" s="0" t="n">
+      <c r="H176" s="1" t="n">
         <v>0.29838467</v>
       </c>
-      <c r="I176" s="0" t="n">
+      <c r="I176" s="1" t="n">
         <v>0.013180733</v>
       </c>
     </row>
@@ -10693,13 +10710,13 @@
       <c r="F177" s="0" t="s">
         <v>1054</v>
       </c>
-      <c r="G177" s="0" t="n">
+      <c r="G177" s="1" t="n">
         <v>1.2200956</v>
       </c>
-      <c r="H177" s="0" t="n">
+      <c r="H177" s="1" t="n">
         <v>0.33126545</v>
       </c>
-      <c r="I177" s="0" t="n">
+      <c r="I177" s="1" t="n">
         <v>0.065223336</v>
       </c>
     </row>
@@ -10722,13 +10739,13 @@
       <c r="F178" s="0" t="s">
         <v>1059</v>
       </c>
-      <c r="G178" s="0" t="n">
+      <c r="G178" s="1" t="n">
         <v>0.41589832</v>
       </c>
-      <c r="H178" s="0" t="n">
+      <c r="H178" s="1" t="n">
         <v>5.220951</v>
       </c>
-      <c r="I178" s="0" t="n">
+      <c r="I178" s="1" t="n">
         <v>0.036191225</v>
       </c>
     </row>
@@ -10751,13 +10768,13 @@
       <c r="F179" s="0" t="s">
         <v>1065</v>
       </c>
-      <c r="G179" s="0" t="n">
+      <c r="G179" s="1" t="n">
         <v>5.2029514</v>
       </c>
-      <c r="H179" s="0" t="n">
+      <c r="H179" s="1" t="n">
         <v>0.14724827</v>
       </c>
-      <c r="I179" s="0" t="n">
+      <c r="I179" s="1" t="n">
         <v>0.11881137</v>
       </c>
     </row>
@@ -10771,7 +10788,7 @@
       <c r="C180" s="0" t="s">
         <v>1068</v>
       </c>
-      <c r="D180" s="1" t="s">
+      <c r="D180" s="2" t="s">
         <v>1069</v>
       </c>
       <c r="E180" s="0" t="s">
@@ -10780,13 +10797,13 @@
       <c r="F180" s="0" t="s">
         <v>1071</v>
       </c>
-      <c r="G180" s="0" t="n">
+      <c r="G180" s="1" t="n">
         <v>1.7054348</v>
       </c>
-      <c r="H180" s="0" t="n">
+      <c r="H180" s="1" t="n">
         <v>1.3689544</v>
       </c>
-      <c r="I180" s="0" t="n">
+      <c r="I180" s="1" t="n">
         <v>0.110845804</v>
       </c>
     </row>
@@ -10809,13 +10826,13 @@
       <c r="F181" s="0" t="s">
         <v>1077</v>
       </c>
-      <c r="G181" s="0" t="n">
+      <c r="G181" s="1" t="n">
         <v>2.839612</v>
       </c>
-      <c r="H181" s="0" t="n">
+      <c r="H181" s="1" t="n">
         <v>0.18058062</v>
       </c>
-      <c r="I181" s="0" t="n">
+      <c r="I181" s="1" t="n">
         <v>0.13369668</v>
       </c>
     </row>
@@ -10838,13 +10855,13 @@
       <c r="F182" s="0" t="s">
         <v>1083</v>
       </c>
-      <c r="G182" s="0" t="n">
+      <c r="G182" s="1" t="n">
         <v>4.3262014</v>
       </c>
-      <c r="H182" s="0" t="n">
+      <c r="H182" s="1" t="n">
         <v>1.0930817</v>
       </c>
-      <c r="I182" s="0" t="n">
+      <c r="I182" s="1" t="n">
         <v>0.11826432</v>
       </c>
     </row>
@@ -10858,7 +10875,7 @@
       <c r="C183" s="0" t="s">
         <v>1086</v>
       </c>
-      <c r="D183" s="1" t="s">
+      <c r="D183" s="2" t="s">
         <v>1087</v>
       </c>
       <c r="E183" s="0" t="s">
@@ -10867,13 +10884,13 @@
       <c r="F183" s="0" t="s">
         <v>1089</v>
       </c>
-      <c r="G183" s="0" t="n">
+      <c r="G183" s="1" t="n">
         <v>4.253955</v>
       </c>
-      <c r="H183" s="0" t="n">
+      <c r="H183" s="1" t="n">
         <v>1.74546</v>
       </c>
-      <c r="I183" s="0" t="n">
+      <c r="I183" s="1" t="n">
         <v>0.07989919</v>
       </c>
     </row>
@@ -10887,7 +10904,7 @@
       <c r="C184" s="0" t="s">
         <v>1092</v>
       </c>
-      <c r="D184" s="1" t="s">
+      <c r="D184" s="2" t="s">
         <v>1093</v>
       </c>
       <c r="E184" s="0" t="s">
@@ -10896,13 +10913,13 @@
       <c r="F184" s="0" t="s">
         <v>1095</v>
       </c>
-      <c r="G184" s="0" t="n">
+      <c r="G184" s="1" t="n">
         <v>7.0499153</v>
       </c>
-      <c r="H184" s="0" t="n">
+      <c r="H184" s="1" t="n">
         <v>2.366712</v>
       </c>
-      <c r="I184" s="0" t="n">
+      <c r="I184" s="1" t="n">
         <v>0.102286816</v>
       </c>
     </row>
@@ -10916,22 +10933,22 @@
       <c r="C185" s="0" t="s">
         <v>1098</v>
       </c>
-      <c r="D185" s="1" t="s">
+      <c r="D185" s="2" t="s">
         <v>1093</v>
       </c>
       <c r="E185" s="0" t="s">
         <v>1099</v>
       </c>
-      <c r="F185" s="1" t="s">
+      <c r="F185" s="2" t="s">
         <v>1100</v>
       </c>
-      <c r="G185" s="0" t="n">
+      <c r="G185" s="1" t="n">
         <v>1.6207342</v>
       </c>
-      <c r="H185" s="0" t="n">
+      <c r="H185" s="1" t="n">
         <v>3.0440946</v>
       </c>
-      <c r="I185" s="0" t="n">
+      <c r="I185" s="1" t="n">
         <v>0.10748923</v>
       </c>
     </row>
@@ -10945,7 +10962,7 @@
       <c r="C186" s="0" t="s">
         <v>1103</v>
       </c>
-      <c r="D186" s="1" t="s">
+      <c r="D186" s="2" t="s">
         <v>1104</v>
       </c>
       <c r="E186" s="0" t="s">
@@ -10954,13 +10971,13 @@
       <c r="F186" s="0" t="s">
         <v>1106</v>
       </c>
-      <c r="G186" s="0" t="n">
+      <c r="G186" s="1" t="n">
         <v>0.8546829</v>
       </c>
-      <c r="H186" s="0" t="n">
+      <c r="H186" s="1" t="n">
         <v>0.23924279</v>
       </c>
-      <c r="I186" s="0" t="n">
+      <c r="I186" s="1" t="n">
         <v>0.10667777</v>
       </c>
     </row>

</xml_diff>